<commit_message>
Primera Versión Completa (mucha cosa, me da susto)
</commit_message>
<xml_diff>
--- a/Ficha_Generica_4.0_-_Multiclase_Update.xlsx
+++ b/Ficha_Generica_4.0_-_Multiclase_Update.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Ficha 1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Magia" sheetId="4" r:id="rId4"/>
     <sheet name="Clase" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1112,7 +1112,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2638,7 +2638,19 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="52" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="48" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="30" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2652,6 +2664,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="52" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2678,21 +2693,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="48" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="31" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="30" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="32" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="71" xfId="2" applyBorder="1" applyAlignment="1">
@@ -3282,7 +3282,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3317,7 +3317,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3530,7 +3530,7 @@
   <dimension ref="C1:DV64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S35" sqref="S35"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4715,36 +4715,96 @@
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="33"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
-      <c r="W11" s="6"/>
-      <c r="X11" s="6"/>
-      <c r="Y11" s="6"/>
-      <c r="Z11" s="6"/>
-      <c r="AA11" s="6"/>
-      <c r="AB11" s="6"/>
-      <c r="AC11" s="6"/>
-      <c r="AD11" s="6"/>
-      <c r="AE11" s="6"/>
-      <c r="AF11" s="6"/>
-      <c r="AG11" s="6"/>
-      <c r="AH11" s="6"/>
-      <c r="AI11" s="6"/>
+      <c r="F11" s="6">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6">
+        <v>2</v>
+      </c>
+      <c r="H11" s="6">
+        <v>3</v>
+      </c>
+      <c r="I11" s="6">
+        <v>4</v>
+      </c>
+      <c r="J11" s="6">
+        <v>45352</v>
+      </c>
+      <c r="K11" s="6">
+        <v>1</v>
+      </c>
+      <c r="L11" s="6">
+        <v>5</v>
+      </c>
+      <c r="M11" s="6">
+        <v>515</v>
+      </c>
+      <c r="N11" s="6">
+        <v>46</v>
+      </c>
+      <c r="O11" s="6">
+        <v>26</v>
+      </c>
+      <c r="P11" s="6">
+        <v>2361</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>1</v>
+      </c>
+      <c r="R11" s="6">
+        <v>5</v>
+      </c>
+      <c r="S11" s="6">
+        <v>656</v>
+      </c>
+      <c r="T11" s="6">
+        <v>4</v>
+      </c>
+      <c r="U11" s="6">
+        <v>452</v>
+      </c>
+      <c r="V11" s="6">
+        <v>6</v>
+      </c>
+      <c r="W11" s="6">
+        <v>256</v>
+      </c>
+      <c r="X11" s="6">
+        <v>3256</v>
+      </c>
+      <c r="Y11" s="6">
+        <v>34526</v>
+      </c>
+      <c r="Z11" s="6">
+        <v>356</v>
+      </c>
+      <c r="AA11" s="6">
+        <v>32</v>
+      </c>
+      <c r="AB11" s="6">
+        <v>632</v>
+      </c>
+      <c r="AC11" s="6">
+        <v>63</v>
+      </c>
+      <c r="AD11" s="6">
+        <v>56</v>
+      </c>
+      <c r="AE11" s="6">
+        <v>56</v>
+      </c>
+      <c r="AF11" s="6">
+        <v>2</v>
+      </c>
+      <c r="AG11" s="6">
+        <v>6</v>
+      </c>
+      <c r="AH11" s="6">
+        <v>526</v>
+      </c>
+      <c r="AI11" s="6">
+        <v>6</v>
+      </c>
       <c r="AJ11" s="2"/>
       <c r="AK11" s="2"/>
       <c r="AL11" s="2"/>
@@ -5088,7 +5148,7 @@
       <c r="BQ13" s="94"/>
       <c r="BR13" s="94">
         <f>P16</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="BS13" s="94"/>
       <c r="BT13" s="92"/>
@@ -5100,7 +5160,7 @@
       <c r="BZ13" s="2"/>
       <c r="CA13" s="94">
         <f>SUM(BP13:BY13)+IF(OR('Ficha 2'!Y5='Ficha 2'!DA43,'Ficha 2'!Y6='Ficha 2'!DA43,'Ficha 2'!Y7='Ficha 2'!DA43,'Ficha 2'!Y8='Ficha 2'!DA43,'Ficha 2'!Y9='Ficha 2'!DA43,'Ficha 2'!Y10='Ficha 2'!DA43,'Ficha 2'!Y11='Ficha 2'!DA43,'Ficha 2'!Y12='Ficha 2'!DA43,'Ficha 2'!Y13='Ficha 2'!DA43,'Ficha 2'!Y14='Ficha 2'!DA43,'Ficha 2'!Y15='Ficha 2'!DA43,'Ficha 2'!Y16='Ficha 2'!DA43),2,0)</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="CB13" s="94"/>
       <c r="CC13" s="8"/>
@@ -5248,7 +5308,7 @@
       <c r="BQ14" s="95"/>
       <c r="BR14" s="95">
         <f>P18</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="BS14" s="95"/>
       <c r="BT14" s="72"/>
@@ -5260,7 +5320,7 @@
       <c r="BZ14" s="2"/>
       <c r="CA14" s="95">
         <f>SUM(BP14:BY14)</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="CB14" s="95"/>
       <c r="CC14" s="8"/>
@@ -5312,7 +5372,9 @@
       <c r="D15" s="33"/>
       <c r="E15" s="33"/>
       <c r="F15" s="33"/>
-      <c r="G15" s="39"/>
+      <c r="G15" s="39">
+        <v>1</v>
+      </c>
       <c r="H15" s="39"/>
       <c r="I15" s="39"/>
       <c r="J15" s="39"/>
@@ -5321,7 +5383,7 @@
       <c r="M15" s="2"/>
       <c r="N15" s="57">
         <f>SUM(G15:L15)+SUM(Clase!AQ9:BI9)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15" s="57"/>
       <c r="P15" s="57">
@@ -5344,7 +5406,7 @@
       <c r="AB15" s="35"/>
       <c r="AC15" s="101">
         <f>SUM(F11:AI11)</f>
-        <v>0</v>
+        <v>89213</v>
       </c>
       <c r="AD15" s="42"/>
       <c r="AE15" s="42">
@@ -5357,7 +5419,7 @@
       <c r="AI15" s="2"/>
       <c r="AJ15" s="42">
         <f>AC15+AE15+AG15+IF('Ficha 2'!Y5='Ficha 2'!DA52,3,0)+IF('Ficha 2'!Y6='Ficha 2'!DA52,3,0)+IF('Ficha 2'!Y7='Ficha 2'!DA52,3,0)+IF('Ficha 2'!Y8='Ficha 2'!DA52,3,0)+IF('Ficha 2'!Y9='Ficha 2'!DA52,3,0)+IF('Ficha 2'!Y10='Ficha 2'!DA52,3,0)+IF('Ficha 2'!Y11='Ficha 2'!DA52,3,0)+IF('Ficha 2'!Y12='Ficha 2'!DA52,3,0)+IF('Ficha 2'!Y13='Ficha 2'!DA52,3,0)+IF('Ficha 2'!Y14='Ficha 2'!DA52,3,0)+IF('Ficha 2'!Y15='Ficha 2'!DA52,3,0)+IF('Ficha 2'!Y16='Ficha 2'!DA52,3,0)</f>
-        <v>0</v>
+        <v>89213</v>
       </c>
       <c r="AK15" s="42"/>
       <c r="AL15" s="103"/>
@@ -5401,7 +5463,7 @@
       <c r="BQ15" s="95"/>
       <c r="BR15" s="95">
         <f>P19</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="BS15" s="95"/>
       <c r="BT15" s="72"/>
@@ -5413,7 +5475,7 @@
       <c r="BZ15" s="2"/>
       <c r="CA15" s="95">
         <f>SUM(BP15:BY15)+IF(OR('Ficha 2'!Y5='Ficha 2'!DA71,'Ficha 2'!Y6='Ficha 2'!DA71,'Ficha 2'!Y7='Ficha 2'!DA71,'Ficha 2'!Y8='Ficha 2'!DA71,'Ficha 2'!Y9='Ficha 2'!DA71,'Ficha 2'!Y10='Ficha 2'!DA71,'Ficha 2'!Y11='Ficha 2'!DA71,'Ficha 2'!Y12='Ficha 2'!DA71,'Ficha 2'!Y13='Ficha 2'!DA71,'Ficha 2'!Y14='Ficha 2'!DA71,'Ficha 2'!Y15='Ficha 2'!DA71,'Ficha 2'!Y16='Ficha 2'!DA71),2,0)</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="CB15" s="95"/>
       <c r="CC15" s="8"/>
@@ -5465,7 +5527,9 @@
       <c r="D16" s="33"/>
       <c r="E16" s="33"/>
       <c r="F16" s="33"/>
-      <c r="G16" s="40"/>
+      <c r="G16" s="40">
+        <v>2</v>
+      </c>
       <c r="H16" s="40"/>
       <c r="I16" s="40"/>
       <c r="J16" s="40"/>
@@ -5474,12 +5538,12 @@
       <c r="M16" s="2"/>
       <c r="N16" s="57">
         <f>SUM(G16:L16)+SUM(Clase!AQ10:BI10)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O16" s="57"/>
       <c r="P16" s="41">
         <f t="shared" ref="P16:P20" si="0">IF(N16&gt;=10,ROUNDDOWN((N16-10)/2,0),ROUNDUP((N16-10)/2,0))</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="Q16" s="41"/>
       <c r="R16" s="2"/>
@@ -5545,7 +5609,7 @@
       <c r="BQ16" s="95"/>
       <c r="BR16" s="95">
         <f>P19</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="BS16" s="95"/>
       <c r="BT16" s="72"/>
@@ -5557,7 +5621,7 @@
       <c r="BZ16" s="2"/>
       <c r="CA16" s="95">
         <f>SUM(BP16:BY16)+IF(OR('Ficha 2'!Y5='Ficha 2'!DA7,'Ficha 2'!Y6='Ficha 2'!DA7,'Ficha 2'!Y7='Ficha 2'!DA7,'Ficha 2'!Y8='Ficha 2'!DA7,'Ficha 2'!Y9='Ficha 2'!DA7,'Ficha 2'!Y10='Ficha 2'!DA7,'Ficha 2'!Y11='Ficha 2'!DA7,'Ficha 2'!Y12='Ficha 2'!DA7,'Ficha 2'!Y13='Ficha 2'!DA7,'Ficha 2'!Y14='Ficha 2'!DA7,'Ficha 2'!Y15='Ficha 2'!DA7,'Ficha 2'!Y16='Ficha 2'!DA7),2,0)</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="CB16" s="95"/>
       <c r="CC16" s="8"/>
@@ -5609,7 +5673,9 @@
       <c r="D17" s="33"/>
       <c r="E17" s="33"/>
       <c r="F17" s="33"/>
-      <c r="G17" s="40"/>
+      <c r="G17" s="40">
+        <v>3</v>
+      </c>
       <c r="H17" s="40"/>
       <c r="I17" s="40"/>
       <c r="J17" s="40"/>
@@ -5618,12 +5684,12 @@
       <c r="M17" s="2"/>
       <c r="N17" s="57">
         <f>SUM(G17:L17)+SUM(Clase!AQ11:BI11)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O17" s="57"/>
       <c r="P17" s="41">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="Q17" s="41"/>
       <c r="R17" s="2"/>
@@ -5687,7 +5753,7 @@
       <c r="BQ17" s="95"/>
       <c r="BR17" s="95">
         <f>P18</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="BS17" s="95"/>
       <c r="BT17" s="72"/>
@@ -5699,7 +5765,7 @@
       <c r="BZ17" s="2"/>
       <c r="CA17" s="95">
         <f>SUM(BP17:BY17)+IF(OR('Ficha 2'!Y5='Ficha 2'!DA66,'Ficha 2'!Y6='Ficha 2'!DA66,'Ficha 2'!Y7='Ficha 2'!DA66,'Ficha 2'!Y8='Ficha 2'!DA66,'Ficha 2'!Y9='Ficha 2'!DA66,'Ficha 2'!Y10='Ficha 2'!DA66,'Ficha 2'!Y11='Ficha 2'!DA66,'Ficha 2'!Y12='Ficha 2'!DA66,'Ficha 2'!Y13='Ficha 2'!DA66,'Ficha 2'!Y14='Ficha 2'!DA66,'Ficha 2'!Y15='Ficha 2'!DA66,'Ficha 2'!Y16='Ficha 2'!DA66),2,0)</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="CB17" s="95"/>
       <c r="CC17" s="8"/>
@@ -5754,7 +5820,9 @@
       <c r="D18" s="33"/>
       <c r="E18" s="33"/>
       <c r="F18" s="33"/>
-      <c r="G18" s="40"/>
+      <c r="G18" s="40">
+        <v>4</v>
+      </c>
       <c r="H18" s="40"/>
       <c r="I18" s="40"/>
       <c r="J18" s="40"/>
@@ -5763,12 +5831,12 @@
       <c r="M18" s="2"/>
       <c r="N18" s="57">
         <f>SUM(G18:L18)+SUM(Clase!AQ12:BI12)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O18" s="57"/>
       <c r="P18" s="41">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="Q18" s="41"/>
       <c r="R18" s="2"/>
@@ -5854,7 +5922,7 @@
       <c r="BQ18" s="95"/>
       <c r="BR18" s="95">
         <f>P17</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="BS18" s="95"/>
       <c r="BT18" s="72"/>
@@ -5866,7 +5934,7 @@
       <c r="BZ18" s="2"/>
       <c r="CA18" s="95">
         <f t="shared" ref="CA18:CA59" si="1">SUM(BP18:BY18)</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="CB18" s="95"/>
       <c r="CC18" s="8"/>
@@ -5918,7 +5986,9 @@
       <c r="D19" s="33"/>
       <c r="E19" s="33"/>
       <c r="F19" s="33"/>
-      <c r="G19" s="40"/>
+      <c r="G19" s="40">
+        <v>5</v>
+      </c>
       <c r="H19" s="40"/>
       <c r="I19" s="40"/>
       <c r="J19" s="40"/>
@@ -5927,12 +5997,12 @@
       <c r="M19" s="2"/>
       <c r="N19" s="57">
         <f>SUM(G19:L19)+SUM(Clase!AQ13:BI13)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O19" s="57"/>
       <c r="P19" s="41">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="Q19" s="41"/>
       <c r="R19" s="2"/>
@@ -6018,7 +6088,7 @@
       <c r="BQ19" s="95"/>
       <c r="BR19" s="95">
         <f>P18</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="BS19" s="95"/>
       <c r="BT19" s="72"/>
@@ -6030,7 +6100,7 @@
       <c r="BZ19" s="2"/>
       <c r="CA19" s="95">
         <f>SUM(BP19:BY19)+CC19+IF(OR('Ficha 2'!Y5='Ficha 2'!DA59,'Ficha 2'!Y6='Ficha 2'!DA59,'Ficha 2'!Y7='Ficha 2'!DA59,'Ficha 2'!Y8='Ficha 2'!DA59,'Ficha 2'!Y9='Ficha 2'!DA59,'Ficha 2'!Y10='Ficha 2'!DA59,'Ficha 2'!Y11='Ficha 2'!DA59,'Ficha 2'!Y12='Ficha 2'!DA59,'Ficha 2'!Y13='Ficha 2'!DA59,'Ficha 2'!Y14='Ficha 2'!DA59,'Ficha 2'!Y15='Ficha 2'!DA59,'Ficha 2'!Y16='Ficha 2'!DA59),2,0)</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="CB19" s="95"/>
       <c r="CC19" s="8">
@@ -6088,7 +6158,9 @@
       <c r="D20" s="33"/>
       <c r="E20" s="33"/>
       <c r="F20" s="33"/>
-      <c r="G20" s="40"/>
+      <c r="G20" s="40">
+        <v>6</v>
+      </c>
       <c r="H20" s="40"/>
       <c r="I20" s="40"/>
       <c r="J20" s="40"/>
@@ -6097,12 +6169,12 @@
       <c r="M20" s="2"/>
       <c r="N20" s="57">
         <f>SUM(G20:L20)+SUM(Clase!AQ14:BI14)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="O20" s="57"/>
       <c r="P20" s="41">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="Q20" s="41"/>
       <c r="R20" s="2"/>
@@ -6131,7 +6203,7 @@
       <c r="AE20" s="42"/>
       <c r="AF20" s="42">
         <f>IF('Ficha 2'!N14=0,'Ficha 1'!P16,IF('Ficha 2'!Q14&gt;='Ficha 1'!P16,'Ficha 1'!P16,'Ficha 2'!Q14))</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="AG20" s="42"/>
       <c r="AH20" s="42">
@@ -6150,12 +6222,12 @@
       <c r="AR20" s="2"/>
       <c r="AS20" s="42">
         <f>SUM(Z20:AQ20)+'Ficha 2'!I27+'Ficha 2'!I33</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AT20" s="42"/>
       <c r="AU20" s="42">
         <f>Z20+SUM(AF20:AI20)+SUM(AL20:AQ20)+'Ficha 2'!I27+'Ficha 2'!I33</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AV20" s="42"/>
       <c r="AW20" s="42">
@@ -6191,7 +6263,7 @@
       <c r="BQ20" s="95"/>
       <c r="BR20" s="95">
         <f>P18</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="BS20" s="95"/>
       <c r="BT20" s="72"/>
@@ -6203,7 +6275,7 @@
       <c r="BZ20" s="2"/>
       <c r="CA20" s="95">
         <f>SUM(BP20:BY20)+IF(OR('Ficha 2'!Y5='Ficha 2'!DA8,'Ficha 2'!Y6='Ficha 2'!DA8,'Ficha 2'!Y7='Ficha 2'!DA8,'Ficha 2'!Y8='Ficha 2'!DA8,'Ficha 2'!Y9='Ficha 2'!DA8,'Ficha 2'!Y10='Ficha 2'!DA8,'Ficha 2'!Y11='Ficha 2'!DA8,'Ficha 2'!Y12='Ficha 2'!DA8,'Ficha 2'!Y13='Ficha 2'!DA8,'Ficha 2'!Y14='Ficha 2'!DA8,'Ficha 2'!Y15='Ficha 2'!DA8,'Ficha 2'!Y16='Ficha 2'!DA8),2,0)</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="CB20" s="95"/>
       <c r="CC20" s="8"/>
@@ -6325,7 +6397,7 @@
       <c r="BQ21" s="95"/>
       <c r="BR21" s="95">
         <f>P20</f>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="BS21" s="95"/>
       <c r="BT21" s="72"/>
@@ -6337,7 +6409,7 @@
       <c r="BZ21" s="2"/>
       <c r="CA21" s="95">
         <f>SUM(BP21:BY21)+CC21+IF(OR('Ficha 2'!Y5='Ficha 2'!DA71,'Ficha 2'!Y6='Ficha 2'!DA71,'Ficha 2'!Y7='Ficha 2'!DA71,'Ficha 2'!Y8='Ficha 2'!DA71,'Ficha 2'!Y9='Ficha 2'!DA71,'Ficha 2'!Y10='Ficha 2'!DA71,'Ficha 2'!Y11='Ficha 2'!DA71,'Ficha 2'!Y12='Ficha 2'!DA71,'Ficha 2'!Y13='Ficha 2'!DA71,'Ficha 2'!Y14='Ficha 2'!DA71,'Ficha 2'!Y15='Ficha 2'!DA71,'Ficha 2'!Y16='Ficha 2'!DA71),2,0)</f>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="CB21" s="95"/>
       <c r="CC21" s="8">
@@ -6488,7 +6560,7 @@
       <c r="BQ22" s="95"/>
       <c r="BR22" s="95">
         <f>P20</f>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="BS22" s="95"/>
       <c r="BT22" s="72"/>
@@ -6500,7 +6572,7 @@
       <c r="BZ22" s="2"/>
       <c r="CA22" s="95">
         <f>SUM(BP22:BY22)+IF(OR('Ficha 2'!Y5='Ficha 2'!DA53,'Ficha 2'!Y6='Ficha 2'!DA53,'Ficha 2'!Y7='Ficha 2'!DA53,'Ficha 2'!Y8='Ficha 2'!DA53,'Ficha 2'!Y9='Ficha 2'!DA53,'Ficha 2'!Y10='Ficha 2'!DA53,'Ficha 2'!Y11='Ficha 2'!DA53,'Ficha 2'!Y12='Ficha 2'!DA53,'Ficha 2'!Y13='Ficha 2'!DA53,'Ficha 2'!Y14='Ficha 2'!DA53,'Ficha 2'!Y15='Ficha 2'!DA53,'Ficha 2'!Y16='Ficha 2'!DA53),2,0)</f>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="CB22" s="95"/>
       <c r="CC22" s="8"/>
@@ -6655,7 +6727,7 @@
       <c r="BQ23" s="95"/>
       <c r="BR23" s="95">
         <f>P20</f>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="BS23" s="95"/>
       <c r="BT23" s="72"/>
@@ -6667,7 +6739,7 @@
       <c r="BZ23" s="2"/>
       <c r="CA23" s="95">
         <f>SUM(BP23:BY23)+IF(OR('Ficha 2'!Y5='Ficha 2'!DA77,'Ficha 2'!Y6='Ficha 2'!DA77,'Ficha 2'!Y7='Ficha 2'!DA77,'Ficha 2'!Y8='Ficha 2'!DA77,'Ficha 2'!Y9='Ficha 2'!DA77,'Ficha 2'!Y10='Ficha 2'!DA77,'Ficha 2'!Y11='Ficha 2'!DA77,'Ficha 2'!Y12='Ficha 2'!DA77,'Ficha 2'!Y13='Ficha 2'!DA77,'Ficha 2'!Y14='Ficha 2'!DA77,'Ficha 2'!Y15='Ficha 2'!DA77,'Ficha 2'!Y16='Ficha 2'!DA77),2,0)</f>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="CB23" s="95"/>
       <c r="CC23" s="8"/>
@@ -6727,7 +6799,7 @@
       <c r="I24" s="41"/>
       <c r="J24" s="42">
         <f>P17</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="K24" s="42"/>
       <c r="L24" s="39"/>
@@ -6739,7 +6811,7 @@
       <c r="R24" s="2"/>
       <c r="S24" s="42">
         <f>H24+J24+L24+N24+P24+IF(OR('Ficha 2'!Y5='Ficha 2'!DA60,'Ficha 2'!Y6='Ficha 2'!DA60,'Ficha 2'!Y7='Ficha 2'!DA60,'Ficha 2'!Y8='Ficha 2'!DA60,'Ficha 2'!Y9='Ficha 2'!DA60,'Ficha 2'!Y10='Ficha 2'!DA60,'Ficha 2'!Y11='Ficha 2'!DA60,'Ficha 2'!Y12='Ficha 2'!DA60,'Ficha 2'!Y13='Ficha 2'!DA60,'Ficha 2'!Y14='Ficha 2'!DA60,'Ficha 2'!Y15='Ficha 2'!DA60,'Ficha 2'!Y16='Ficha 2'!DA60),2,0)</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="T24" s="42"/>
       <c r="U24" s="2"/>
@@ -6752,7 +6824,7 @@
       <c r="Z24" s="33"/>
       <c r="AA24" s="42">
         <f>P16</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="AB24" s="42"/>
       <c r="AC24" s="88"/>
@@ -6762,7 +6834,7 @@
       <c r="AG24" s="2"/>
       <c r="AH24" s="42">
         <f>SUM(AA24:AF24)+IF(OR('Ficha 2'!Y5='Ficha 2'!DA65,'Ficha 2'!Y6='Ficha 2'!DA65,'Ficha 2'!Y7='Ficha 2'!DA65,'Ficha 2'!Y8='Ficha 2'!DA65,'Ficha 2'!Y9='Ficha 2'!DA65,'Ficha 2'!Y10='Ficha 2'!DA65,'Ficha 2'!Y11='Ficha 2'!DA65,'Ficha 2'!Y12='Ficha 2'!DA65,'Ficha 2'!Y13='Ficha 2'!DA65,'Ficha 2'!Y14='Ficha 2'!DA65,'Ficha 2'!Y15='Ficha 2'!DA65,'Ficha 2'!Y16='Ficha 2'!DA65),4,0)</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="AI24" s="42"/>
       <c r="AJ24" s="2"/>
@@ -6813,7 +6885,7 @@
       <c r="BQ24" s="95"/>
       <c r="BR24" s="95">
         <f>P16</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="BS24" s="95"/>
       <c r="BT24" s="72"/>
@@ -6828,7 +6900,7 @@
       <c r="BZ24" s="2"/>
       <c r="CA24" s="95">
         <f>SUM(BP24:BY24)+CC24+IF(OR('Ficha 2'!Y5='Ficha 2'!DA4,'Ficha 2'!Y6='Ficha 2'!DA4,'Ficha 2'!Y7='Ficha 2'!DA4,'Ficha 2'!Y8='Ficha 2'!DA4,'Ficha 2'!Y9='Ficha 2'!DA4,'Ficha 2'!Y10='Ficha 2'!DA4,'Ficha 2'!Y11='Ficha 2'!DA4,'Ficha 2'!Y12='Ficha 2'!DA4,'Ficha 2'!Y13='Ficha 2'!DA4,'Ficha 2'!Y14='Ficha 2'!DA4,'Ficha 2'!Y15='Ficha 2'!DA4,'Ficha 2'!Y16='Ficha 2'!DA4),2,0)</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="CB24" s="95"/>
       <c r="CC24" s="8">
@@ -6891,7 +6963,7 @@
       <c r="I25" s="41"/>
       <c r="J25" s="43">
         <f>P16</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="K25" s="43"/>
       <c r="L25" s="40"/>
@@ -6903,7 +6975,7 @@
       <c r="R25" s="2"/>
       <c r="S25" s="43">
         <f>H25+J25+L25+N25+P25+IF(OR('Ficha 2'!Y5='Ficha 2'!DA81,'Ficha 2'!Y6='Ficha 2'!DA81,'Ficha 2'!Y7='Ficha 2'!DA81,'Ficha 2'!Y8='Ficha 2'!DA81,'Ficha 2'!Y9='Ficha 2'!DA81,'Ficha 2'!Y10='Ficha 2'!DA81,'Ficha 2'!Y11='Ficha 2'!DA81,'Ficha 2'!Y12='Ficha 2'!DA81,'Ficha 2'!Y13='Ficha 2'!DA81,'Ficha 2'!Y14='Ficha 2'!DA81,'Ficha 2'!Y15='Ficha 2'!DA81,'Ficha 2'!Y16='Ficha 2'!DA81),2,0)</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="T25" s="43"/>
       <c r="U25" s="2"/>
@@ -6964,7 +7036,7 @@
       <c r="BQ25" s="95"/>
       <c r="BR25" s="95">
         <f>P16</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="BS25" s="95"/>
       <c r="BT25" s="72"/>
@@ -6979,7 +7051,7 @@
       <c r="BZ25" s="2"/>
       <c r="CA25" s="95">
         <f>SUM(BP25:BY25)+IF(OR('Ficha 2'!Y5='Ficha 2'!DA4,'Ficha 2'!Y6='Ficha 2'!DA4,'Ficha 2'!Y7='Ficha 2'!DA4,'Ficha 2'!Y8='Ficha 2'!DA4,'Ficha 2'!Y9='Ficha 2'!DA4,'Ficha 2'!Y10='Ficha 2'!DA4,'Ficha 2'!Y11='Ficha 2'!DA4,'Ficha 2'!Y12='Ficha 2'!DA4,'Ficha 2'!Y13='Ficha 2'!DA4,'Ficha 2'!Y14='Ficha 2'!DA4,'Ficha 2'!Y15='Ficha 2'!DA4,'Ficha 2'!Y16='Ficha 2'!DA4),2,0)</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="CB25" s="95"/>
       <c r="CC25" s="8"/>
@@ -7042,7 +7114,7 @@
       <c r="I26" s="41"/>
       <c r="J26" s="43">
         <f>P19</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="K26" s="43"/>
       <c r="L26" s="40"/>
@@ -7054,7 +7126,7 @@
       <c r="R26" s="2"/>
       <c r="S26" s="43">
         <f>H26+J26+L26+N26+P26+IF(OR('Ficha 2'!Y5='Ficha 2'!DA91,'Ficha 2'!Y6='Ficha 2'!DA91,'Ficha 2'!Y7='Ficha 2'!DA91,'Ficha 2'!Y8='Ficha 2'!DA91,'Ficha 2'!Y9='Ficha 2'!DA91,'Ficha 2'!Y10='Ficha 2'!DA91,'Ficha 2'!Y11='Ficha 2'!DA91,'Ficha 2'!Y12='Ficha 2'!DA91,'Ficha 2'!Y13='Ficha 2'!DA91,'Ficha 2'!Y14='Ficha 2'!DA91,'Ficha 2'!Y15='Ficha 2'!DA91,'Ficha 2'!Y16='Ficha 2'!DA91),2,0)</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="T26" s="43"/>
       <c r="U26" s="2"/>
@@ -7119,7 +7191,7 @@
       <c r="BQ26" s="95"/>
       <c r="BR26" s="95">
         <f>P16</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="BS26" s="95"/>
       <c r="BT26" s="72"/>
@@ -7134,7 +7206,7 @@
       <c r="BZ26" s="2"/>
       <c r="CA26" s="95">
         <f>SUM(BP26:BY26)+IF(OR('Ficha 2'!Y5='Ficha 2'!DA82,'Ficha 2'!Y6='Ficha 2'!DA82,'Ficha 2'!Y7='Ficha 2'!DA82,'Ficha 2'!Y8='Ficha 2'!DA82,'Ficha 2'!Y9='Ficha 2'!DA82,'Ficha 2'!Y10='Ficha 2'!DA82,'Ficha 2'!Y11='Ficha 2'!DA82,'Ficha 2'!Y12='Ficha 2'!DA82,'Ficha 2'!Y13='Ficha 2'!DA82,'Ficha 2'!Y14='Ficha 2'!DA82,'Ficha 2'!Y15='Ficha 2'!DA82,'Ficha 2'!Y16='Ficha 2'!DA82),2,0)</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="CB26" s="95"/>
       <c r="CC26" s="8"/>
@@ -7259,7 +7331,7 @@
       <c r="BQ27" s="95"/>
       <c r="BR27" s="95">
         <f>P19</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="BS27" s="95"/>
       <c r="BT27" s="72"/>
@@ -7271,7 +7343,7 @@
       <c r="BZ27" s="2"/>
       <c r="CA27" s="95">
         <f>SUM(BP27:BY27)+IF(OR('Ficha 2'!Y5='Ficha 2'!DA7,'Ficha 2'!Y6='Ficha 2'!DA7,'Ficha 2'!Y7='Ficha 2'!DA7,'Ficha 2'!Y8='Ficha 2'!DA7,'Ficha 2'!Y9='Ficha 2'!DA7,'Ficha 2'!Y10='Ficha 2'!DA7,'Ficha 2'!Y11='Ficha 2'!DA7,'Ficha 2'!Y12='Ficha 2'!DA7,'Ficha 2'!Y13='Ficha 2'!DA7,'Ficha 2'!Y14='Ficha 2'!DA7,'Ficha 2'!Y15='Ficha 2'!DA7,'Ficha 2'!Y16='Ficha 2'!DA7),2,0)</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="CB27" s="95"/>
       <c r="CC27" s="8"/>
@@ -7411,7 +7483,7 @@
       <c r="BQ28" s="95"/>
       <c r="BR28" s="95">
         <f>P18</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="BS28" s="95"/>
       <c r="BT28" s="72"/>
@@ -7423,7 +7495,7 @@
       <c r="BZ28" s="2"/>
       <c r="CA28" s="95">
         <f>SUM(BP28:BY28)+IF(OR('Ficha 2'!Y5='Ficha 2'!DA53,'Ficha 2'!Y6='Ficha 2'!DA53,'Ficha 2'!Y7='Ficha 2'!DA53,'Ficha 2'!Y8='Ficha 2'!DA53,'Ficha 2'!Y9='Ficha 2'!DA53,'Ficha 2'!Y10='Ficha 2'!DA53,'Ficha 2'!Y11='Ficha 2'!DA53,'Ficha 2'!Y12='Ficha 2'!DA53,'Ficha 2'!Y13='Ficha 2'!DA53,'Ficha 2'!Y14='Ficha 2'!DA53,'Ficha 2'!Y15='Ficha 2'!DA53,'Ficha 2'!Y16='Ficha 2'!DA53),2,0)</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="CB28" s="95"/>
       <c r="CC28" s="8"/>
@@ -7547,7 +7619,7 @@
       <c r="BQ29" s="95"/>
       <c r="BR29" s="95">
         <f>P20</f>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="BS29" s="95"/>
       <c r="BT29" s="72"/>
@@ -7559,7 +7631,7 @@
       <c r="BZ29" s="2"/>
       <c r="CA29" s="95">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="CB29" s="95"/>
       <c r="CC29" s="8"/>
@@ -7689,7 +7761,7 @@
       <c r="BQ30" s="95"/>
       <c r="BR30" s="95">
         <f>P20</f>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="BS30" s="95"/>
       <c r="BT30" s="72"/>
@@ -7701,7 +7773,7 @@
       <c r="BZ30" s="2"/>
       <c r="CA30" s="95">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="CB30" s="95"/>
       <c r="CC30" s="8"/>
@@ -7826,7 +7898,7 @@
       <c r="BQ31" s="95"/>
       <c r="BR31" s="95">
         <f>P20</f>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="BS31" s="95"/>
       <c r="BT31" s="72"/>
@@ -7838,7 +7910,7 @@
       <c r="BZ31" s="2"/>
       <c r="CA31" s="95">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="CB31" s="95"/>
       <c r="CC31" s="8"/>
@@ -8123,7 +8195,7 @@
       <c r="BQ33" s="95"/>
       <c r="BR33" s="95">
         <f>P18</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="BS33" s="95"/>
       <c r="BT33" s="72"/>
@@ -8135,7 +8207,7 @@
       <c r="BZ33" s="2"/>
       <c r="CA33" s="95">
         <f>SUM(BP33:BY33)+IF(OR('Ficha 2'!Y5='Ficha 2'!DA43,'Ficha 2'!Y6='Ficha 2'!DA43,'Ficha 2'!Y7='Ficha 2'!DA43,'Ficha 2'!Y8='Ficha 2'!DA43,'Ficha 2'!Y9='Ficha 2'!DA43,'Ficha 2'!Y10='Ficha 2'!DA43,'Ficha 2'!Y11='Ficha 2'!DA43,'Ficha 2'!Y12='Ficha 2'!DA43,'Ficha 2'!Y13='Ficha 2'!DA43,'Ficha 2'!Y14='Ficha 2'!DA43,'Ficha 2'!Y15='Ficha 2'!DA43,'Ficha 2'!Y16='Ficha 2'!DA43),2,0)</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="CB33" s="95"/>
       <c r="CC33" s="8"/>
@@ -8272,7 +8344,7 @@
       <c r="BQ34" s="95"/>
       <c r="BR34" s="95">
         <f>P16</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="BS34" s="95"/>
       <c r="BT34" s="72"/>
@@ -8284,7 +8356,7 @@
       <c r="BZ34" s="2"/>
       <c r="CA34" s="95">
         <f>SUM(BP34:BY34)+CC34+IF(OR('Ficha 2'!Y5='Ficha 2'!DA70,'Ficha 2'!Y6='Ficha 2'!DA70,'Ficha 2'!Y7='Ficha 2'!DA70,'Ficha 2'!Y8='Ficha 2'!DA70,'Ficha 2'!Y9='Ficha 2'!DA70,'Ficha 2'!Y10='Ficha 2'!DA70,'Ficha 2'!Y11='Ficha 2'!DA70,'Ficha 2'!Y12='Ficha 2'!DA70,'Ficha 2'!Y13='Ficha 2'!DA70,'Ficha 2'!Y14='Ficha 2'!DA70,'Ficha 2'!Y15='Ficha 2'!DA70,'Ficha 2'!Y16='Ficha 2'!DA70),2,0)</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="CB34" s="95"/>
       <c r="CC34" s="8">
@@ -8412,7 +8484,7 @@
       <c r="BQ35" s="95"/>
       <c r="BR35" s="95">
         <f>P16</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="BS35" s="95"/>
       <c r="BT35" s="72"/>
@@ -8424,7 +8496,7 @@
       <c r="BZ35" s="2"/>
       <c r="CA35" s="95">
         <f>SUM(BP35:BY35)+CC35+IF(OR('Ficha 2'!Y5='Ficha 2'!DA3,'Ficha 2'!Y6='Ficha 2'!DA3,'Ficha 2'!Y7='Ficha 2'!DA3,'Ficha 2'!Y8='Ficha 2'!DA3,'Ficha 2'!Y9='Ficha 2'!DA3,'Ficha 2'!Y10='Ficha 2'!DA3,'Ficha 2'!Y11='Ficha 2'!DA3,'Ficha 2'!Y12='Ficha 2'!DA3,'Ficha 2'!Y13='Ficha 2'!DA3,'Ficha 2'!Y14='Ficha 2'!DA3,'Ficha 2'!Y15='Ficha 2'!DA3,'Ficha 2'!Y16='Ficha 2'!DA3),2,0)</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="CB35" s="95"/>
       <c r="CC35" s="8">
@@ -8562,7 +8634,7 @@
       <c r="BQ36" s="95"/>
       <c r="BR36" s="95">
         <f>P16</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="BS36" s="95"/>
       <c r="BT36" s="72"/>
@@ -8577,7 +8649,7 @@
       <c r="BZ36" s="2"/>
       <c r="CA36" s="95">
         <f>SUM(BP36:BY36)+IF(OR('Ficha 2'!Y5='Ficha 2'!DA82,'Ficha 2'!Y6='Ficha 2'!DA82,'Ficha 2'!Y7='Ficha 2'!DA82,'Ficha 2'!Y8='Ficha 2'!DA82,'Ficha 2'!Y9='Ficha 2'!DA82,'Ficha 2'!Y10='Ficha 2'!DA82,'Ficha 2'!Y11='Ficha 2'!DA82,'Ficha 2'!Y12='Ficha 2'!DA82,'Ficha 2'!Y13='Ficha 2'!DA82,'Ficha 2'!Y14='Ficha 2'!DA82,'Ficha 2'!Y15='Ficha 2'!DA82,'Ficha 2'!Y16='Ficha 2'!DA82),2,0)</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="CB36" s="95"/>
       <c r="CC36" s="8"/>
@@ -8881,7 +8953,7 @@
       <c r="BQ38" s="95"/>
       <c r="BR38" s="95">
         <f>IF(BL38=C15,P15,0)+IF(BL38=C16,P16,0)+IF(BL38=C17,P17,0)+IF(BL38=C18,P18,0)+IF(BL38=C19,P19,0)+IF(BL38=C20,P20,0)</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="BS38" s="95"/>
       <c r="BT38" s="72"/>
@@ -8893,7 +8965,7 @@
       <c r="BZ38" s="2"/>
       <c r="CA38" s="95">
         <f>SUM(BP38:BY38)</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="CB38" s="95"/>
       <c r="CC38" s="8"/>
@@ -9023,7 +9095,7 @@
       <c r="BQ39" s="95"/>
       <c r="BR39" s="95">
         <f>P16</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="BS39" s="95"/>
       <c r="BT39" s="72"/>
@@ -9038,7 +9110,7 @@
       <c r="BZ39" s="2"/>
       <c r="CA39" s="95">
         <f>SUM(BP39:BY39)+CC39+IF(OR('Ficha 2'!Y5='Ficha 2'!DA2,'Ficha 2'!Y6='Ficha 2'!DA2,'Ficha 2'!Y7='Ficha 2'!DA2,'Ficha 2'!Y8='Ficha 2'!DA2,'Ficha 2'!Y9='Ficha 2'!DA2,'Ficha 2'!Y10='Ficha 2'!DA2,'Ficha 2'!Y11='Ficha 2'!DA2,'Ficha 2'!Y12='Ficha 2'!DA2,'Ficha 2'!Y13='Ficha 2'!DA2,'Ficha 2'!Y14='Ficha 2'!DA2,'Ficha 2'!Y15='Ficha 2'!DA2,'Ficha 2'!Y16='Ficha 2'!DA2),2,0)</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="CB39" s="95"/>
       <c r="CC39" s="8">
@@ -9163,7 +9235,7 @@
       <c r="BQ40" s="95"/>
       <c r="BR40" s="95">
         <f>P20</f>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="BS40" s="95"/>
       <c r="BT40" s="72"/>
@@ -9175,7 +9247,7 @@
       <c r="BZ40" s="2"/>
       <c r="CA40" s="95">
         <f>SUM(BP40:BY40)+CC40+IF(OR('Ficha 2'!Y5='Ficha 2'!DA66,'Ficha 2'!Y6='Ficha 2'!DA66,'Ficha 2'!Y7='Ficha 2'!DA66,'Ficha 2'!Y8='Ficha 2'!DA66,'Ficha 2'!Y9='Ficha 2'!DA66,'Ficha 2'!Y10='Ficha 2'!DA66,'Ficha 2'!Y11='Ficha 2'!DA66,'Ficha 2'!Y12='Ficha 2'!DA66,'Ficha 2'!Y13='Ficha 2'!DA66,'Ficha 2'!Y14='Ficha 2'!DA66,'Ficha 2'!Y15='Ficha 2'!DA66,'Ficha 2'!Y16='Ficha 2'!DA66),2,0)</f>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="CB40" s="95"/>
       <c r="CC40" s="8">
@@ -9300,7 +9372,7 @@
       <c r="BQ41" s="95"/>
       <c r="BR41" s="95">
         <f>P18</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="BS41" s="95"/>
       <c r="BT41" s="72"/>
@@ -9312,7 +9384,7 @@
       <c r="BZ41" s="2"/>
       <c r="CA41" s="95">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="CB41" s="95"/>
       <c r="CC41" s="8"/>
@@ -9444,7 +9516,7 @@
       <c r="BQ42" s="95"/>
       <c r="BR42" s="95">
         <f>P18</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="BS42" s="95"/>
       <c r="BT42" s="72"/>
@@ -9456,7 +9528,7 @@
       <c r="BZ42" s="2"/>
       <c r="CA42" s="95">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="CB42" s="95"/>
       <c r="CC42" s="8"/>
@@ -9602,7 +9674,7 @@
       <c r="BQ43" s="95"/>
       <c r="BR43" s="95">
         <f>P18</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="BS43" s="95"/>
       <c r="BT43" s="72"/>
@@ -9614,7 +9686,7 @@
       <c r="BZ43" s="2"/>
       <c r="CA43" s="95">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="CB43" s="95"/>
       <c r="CC43" s="8"/>
@@ -9751,7 +9823,7 @@
       <c r="BQ44" s="95"/>
       <c r="BR44" s="95">
         <f>P18</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="BS44" s="95"/>
       <c r="BT44" s="72"/>
@@ -9763,7 +9835,7 @@
       <c r="BZ44" s="2"/>
       <c r="CA44" s="95">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="CB44" s="95"/>
       <c r="CC44" s="8"/>
@@ -9893,7 +9965,7 @@
       <c r="BQ45" s="95"/>
       <c r="BR45" s="95">
         <f>P18</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="BS45" s="95"/>
       <c r="BT45" s="72"/>
@@ -9905,7 +9977,7 @@
       <c r="BZ45" s="2"/>
       <c r="CA45" s="95">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="CB45" s="95"/>
       <c r="CC45" s="8"/>
@@ -10027,7 +10099,7 @@
       <c r="BQ46" s="95"/>
       <c r="BR46" s="95">
         <f>P18</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="BS46" s="95"/>
       <c r="BT46" s="72"/>
@@ -10039,7 +10111,7 @@
       <c r="BZ46" s="2"/>
       <c r="CA46" s="95">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="CB46" s="95"/>
       <c r="CC46" s="8"/>
@@ -10161,7 +10233,7 @@
       <c r="BQ47" s="95"/>
       <c r="BR47" s="95">
         <f>P18</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="BS47" s="95"/>
       <c r="BT47" s="72"/>
@@ -10173,7 +10245,7 @@
       <c r="BZ47" s="2"/>
       <c r="CA47" s="95">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="CB47" s="95"/>
       <c r="CC47" s="8"/>
@@ -10305,7 +10377,7 @@
       <c r="BQ48" s="95"/>
       <c r="BR48" s="95">
         <f>P18</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="BS48" s="95"/>
       <c r="BT48" s="72"/>
@@ -10317,7 +10389,7 @@
       <c r="BZ48" s="2"/>
       <c r="CA48" s="95">
         <f>SUM(BP48:BY48)+CC48</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="CB48" s="95"/>
       <c r="CC48" s="8">
@@ -10466,7 +10538,7 @@
       <c r="BQ49" s="95"/>
       <c r="BR49" s="95">
         <f>P18</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="BS49" s="95"/>
       <c r="BT49" s="72"/>
@@ -10478,7 +10550,7 @@
       <c r="BZ49" s="2"/>
       <c r="CA49" s="95">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="CB49" s="95"/>
       <c r="CC49" s="8"/>
@@ -10615,7 +10687,7 @@
       <c r="BQ50" s="95"/>
       <c r="BR50" s="95">
         <f>P18</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="BS50" s="95"/>
       <c r="BT50" s="72"/>
@@ -10627,7 +10699,7 @@
       <c r="BZ50" s="2"/>
       <c r="CA50" s="95">
         <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="CB50" s="95"/>
       <c r="CC50" s="8"/>
@@ -10897,7 +10969,7 @@
       <c r="BQ52" s="95"/>
       <c r="BR52" s="95">
         <f>P19</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="BS52" s="95"/>
       <c r="BT52" s="72"/>
@@ -10909,7 +10981,7 @@
       <c r="BZ52" s="2"/>
       <c r="CA52" s="95">
         <f>SUM(BP52:BY52)+IF(OR('Ficha 2'!Y5='Ficha 2'!DA17,'Ficha 2'!Y6='Ficha 2'!DA17,'Ficha 2'!Y7='Ficha 2'!DA17,'Ficha 2'!Y8='Ficha 2'!DA17,'Ficha 2'!Y9='Ficha 2'!DA17,'Ficha 2'!Y10='Ficha 2'!DA17,'Ficha 2'!Y11='Ficha 2'!DA17,'Ficha 2'!Y12='Ficha 2'!DA17,'Ficha 2'!Y13='Ficha 2'!DA17,'Ficha 2'!Y14='Ficha 2'!DA17,'Ficha 2'!Y15='Ficha 2'!DA17,'Ficha 2'!Y16='Ficha 2'!DA17),2,0)</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="CB52" s="95"/>
       <c r="CC52" s="8"/>
@@ -11031,7 +11103,7 @@
       <c r="BQ53" s="95"/>
       <c r="BR53" s="95">
         <f>P19</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="BS53" s="95"/>
       <c r="BT53" s="72"/>
@@ -11043,7 +11115,7 @@
       <c r="BZ53" s="2"/>
       <c r="CA53" s="95">
         <f>SUM(BP53:BY53)+IF(OR('Ficha 2'!Y5='Ficha 2'!DA17,'Ficha 2'!Y6='Ficha 2'!DA17,'Ficha 2'!Y7='Ficha 2'!DA17,'Ficha 2'!Y8='Ficha 2'!DA17,'Ficha 2'!Y9='Ficha 2'!DA17,'Ficha 2'!Y10='Ficha 2'!DA17,'Ficha 2'!Y11='Ficha 2'!DA17,'Ficha 2'!Y12='Ficha 2'!DA17,'Ficha 2'!Y13='Ficha 2'!DA17,'Ficha 2'!Y14='Ficha 2'!DA17,'Ficha 2'!Y15='Ficha 2'!DA17,'Ficha 2'!Y16='Ficha 2'!DA17),2,0)</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="CB53" s="95"/>
       <c r="CC53" s="8"/>
@@ -11178,7 +11250,7 @@
       <c r="BQ54" s="95"/>
       <c r="BR54" s="95">
         <f>P18</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="BS54" s="95"/>
       <c r="BT54" s="72"/>
@@ -11190,7 +11262,7 @@
       <c r="BZ54" s="2"/>
       <c r="CA54" s="95">
         <f>SUM(BP54:BY54)+IF(OR('Ficha 2'!Y5='Ficha 2'!DA8,'Ficha 2'!Y6='Ficha 2'!DA8,'Ficha 2'!Y7='Ficha 2'!DA8,'Ficha 2'!Y8='Ficha 2'!DA8,'Ficha 2'!Y9='Ficha 2'!DA8,'Ficha 2'!Y10='Ficha 2'!DA8,'Ficha 2'!Y11='Ficha 2'!DA8,'Ficha 2'!Y12='Ficha 2'!DA8,'Ficha 2'!Y13='Ficha 2'!DA8,'Ficha 2'!Y14='Ficha 2'!DA8,'Ficha 2'!Y15='Ficha 2'!DA8,'Ficha 2'!Y16='Ficha 2'!DA8),2,0)</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="CB54" s="95"/>
       <c r="CC54" s="8"/>
@@ -11339,7 +11411,7 @@
       <c r="BQ55" s="95"/>
       <c r="BR55" s="95">
         <f>P20</f>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="BS55" s="95"/>
       <c r="BT55" s="72"/>
@@ -11351,7 +11423,7 @@
       <c r="BZ55" s="2"/>
       <c r="CA55" s="95">
         <f>SUM(BP55:BY55)+IF(OR('Ficha 2'!Y5='Ficha 2'!DA3,'Ficha 2'!Y6='Ficha 2'!DA3,'Ficha 2'!Y7='Ficha 2'!DA3,'Ficha 2'!Y8='Ficha 2'!DA3,'Ficha 2'!Y9='Ficha 2'!DA3,'Ficha 2'!Y10='Ficha 2'!DA3,'Ficha 2'!Y11='Ficha 2'!DA3,'Ficha 2'!Y12='Ficha 2'!DA3,'Ficha 2'!Y13='Ficha 2'!DA3,'Ficha 2'!Y14='Ficha 2'!DA3,'Ficha 2'!Y15='Ficha 2'!DA3,'Ficha 2'!Y16='Ficha 2'!DA3),2,0)</f>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="CB55" s="95"/>
       <c r="CC55" s="8"/>
@@ -11488,7 +11560,7 @@
       <c r="BQ56" s="95"/>
       <c r="BR56" s="95">
         <f>IF(OR(BL56=C15,BL56=C16),IF(BL56=C15,P15,P16))</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="BS56" s="95"/>
       <c r="BT56" s="72"/>
@@ -11500,7 +11572,7 @@
       <c r="BZ56" s="2"/>
       <c r="CA56" s="95">
         <f>SUM(BP56:BY56)+IF(OR('Ficha 2'!Y5='Ficha 2'!DA15,'Ficha 2'!Y6='Ficha 2'!DA15,'Ficha 2'!Y7='Ficha 2'!DA15,'Ficha 2'!Y8='Ficha 2'!DA15,'Ficha 2'!Y9='Ficha 2'!DA15,'Ficha 2'!Y10='Ficha 2'!DA15,'Ficha 2'!Y11='Ficha 2'!DA15,'Ficha 2'!Y12='Ficha 2'!DA15,'Ficha 2'!Y13='Ficha 2'!DA15,'Ficha 2'!Y14='Ficha 2'!DA15,'Ficha 2'!Y15='Ficha 2'!DA15,'Ficha 2'!Y16='Ficha 2'!DA15),2,0)</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="CB56" s="95"/>
       <c r="CC56" s="8"/>
@@ -11633,7 +11705,7 @@
       <c r="BQ57" s="95"/>
       <c r="BR57" s="95">
         <f>IF(OR(BL57=C18,BL57=C20),IF(BL57=C18,P18,P20))</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="BS57" s="95"/>
       <c r="BT57" s="72"/>
@@ -11645,7 +11717,7 @@
       <c r="BZ57" s="2"/>
       <c r="CA57" s="95">
         <f>SUM(BP57:BY57)+IF(OR('Ficha 2'!Y5='Ficha 2'!DA59,'Ficha 2'!Y6='Ficha 2'!DA59,'Ficha 2'!Y7='Ficha 2'!DA59,'Ficha 2'!Y8='Ficha 2'!DA59,'Ficha 2'!Y9='Ficha 2'!DA59,'Ficha 2'!Y10='Ficha 2'!DA59,'Ficha 2'!Y11='Ficha 2'!DA59,'Ficha 2'!Y12='Ficha 2'!DA59,'Ficha 2'!Y13='Ficha 2'!DA59,'Ficha 2'!Y14='Ficha 2'!DA59,'Ficha 2'!Y15='Ficha 2'!DA59,'Ficha 2'!Y16='Ficha 2'!DA59),2,0)</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="CB57" s="95"/>
       <c r="CC57" s="8"/>
@@ -11770,7 +11842,7 @@
       <c r="BQ58" s="95"/>
       <c r="BR58" s="95">
         <f>P16</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="BS58" s="95"/>
       <c r="BT58" s="72"/>
@@ -11782,7 +11854,7 @@
       <c r="BZ58" s="2"/>
       <c r="CA58" s="95">
         <f>SUM(BP58:BY58)+IF(OR('Ficha 2'!Y5='Ficha 2'!DA70,'Ficha 2'!Y6='Ficha 2'!DA70,'Ficha 2'!Y7='Ficha 2'!DA70,'Ficha 2'!Y8='Ficha 2'!DA70,'Ficha 2'!Y9='Ficha 2'!DA70,'Ficha 2'!Y10='Ficha 2'!DA70,'Ficha 2'!Y11='Ficha 2'!DA70,'Ficha 2'!Y12='Ficha 2'!DA70,'Ficha 2'!Y13='Ficha 2'!DA70,'Ficha 2'!Y14='Ficha 2'!DA70,'Ficha 2'!Y15='Ficha 2'!DA70,'Ficha 2'!Y16='Ficha 2'!DA70),2,0)</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="CB58" s="95"/>
       <c r="CC58" s="8"/>
@@ -12325,7 +12397,7 @@
       <c r="BL62" s="33"/>
       <c r="BM62" s="100">
         <f>((Clase!AD10+P18)*(3+M5))+IF(Clase!B14=0,0,(Clase!AD20+P18)*(3+M5))+IF(Clase!B24=0,0,(Clase!AD30+P18)*(3+M5))+IF(Clase!B34=0,0,(Clase!AD40+P18)*(3+M5))</f>
-        <v>-15</v>
+        <v>-9</v>
       </c>
       <c r="BN62" s="100"/>
       <c r="BO62" s="2"/>
@@ -27425,7 +27497,7 @@
   <dimension ref="B1:DC40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AM16" sqref="AM16"/>
+      <selection activeCell="Y4" sqref="Y4:AB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27447,22 +27519,22 @@
       </c>
     </row>
     <row r="2" spans="2:107" x14ac:dyDescent="0.25">
-      <c r="Y2" s="166" t="s">
+      <c r="Y2" s="153" t="s">
         <v>337</v>
       </c>
-      <c r="Z2" s="166"/>
-      <c r="AA2" s="166"/>
-      <c r="AB2" s="166"/>
-      <c r="AC2" s="166"/>
-      <c r="AD2" s="166"/>
-      <c r="AE2" s="166"/>
-      <c r="AF2" s="166"/>
-      <c r="AG2" s="166"/>
-      <c r="AH2" s="166"/>
-      <c r="AI2" s="166"/>
-      <c r="AJ2" s="166"/>
-      <c r="AK2" s="166"/>
-      <c r="AL2" s="167"/>
+      <c r="Z2" s="153"/>
+      <c r="AA2" s="153"/>
+      <c r="AB2" s="153"/>
+      <c r="AC2" s="153"/>
+      <c r="AD2" s="153"/>
+      <c r="AE2" s="153"/>
+      <c r="AF2" s="153"/>
+      <c r="AG2" s="153"/>
+      <c r="AH2" s="153"/>
+      <c r="AI2" s="153"/>
+      <c r="AJ2" s="153"/>
+      <c r="AK2" s="153"/>
+      <c r="AL2" s="154"/>
       <c r="AO2" s="145" t="s">
         <v>332</v>
       </c>
@@ -27663,65 +27735,65 @@
       </c>
     </row>
     <row r="5" spans="2:107" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="I5" s="157" t="s">
+      <c r="I5" s="162" t="s">
         <v>345</v>
       </c>
-      <c r="J5" s="158"/>
-      <c r="K5" s="158"/>
-      <c r="L5" s="158"/>
-      <c r="M5" s="158"/>
-      <c r="N5" s="158"/>
-      <c r="O5" s="158"/>
-      <c r="P5" s="159"/>
-      <c r="Q5" s="157" t="s">
+      <c r="J5" s="163"/>
+      <c r="K5" s="163"/>
+      <c r="L5" s="163"/>
+      <c r="M5" s="163"/>
+      <c r="N5" s="163"/>
+      <c r="O5" s="163"/>
+      <c r="P5" s="164"/>
+      <c r="Q5" s="162" t="s">
         <v>336</v>
       </c>
-      <c r="R5" s="158"/>
-      <c r="S5" s="158"/>
-      <c r="T5" s="158"/>
-      <c r="U5" s="158"/>
-      <c r="V5" s="158"/>
-      <c r="W5" s="158"/>
-      <c r="X5" s="159"/>
-      <c r="Y5" s="160" t="s">
+      <c r="R5" s="163"/>
+      <c r="S5" s="163"/>
+      <c r="T5" s="163"/>
+      <c r="U5" s="163"/>
+      <c r="V5" s="163"/>
+      <c r="W5" s="163"/>
+      <c r="X5" s="164"/>
+      <c r="Y5" s="165" t="s">
         <v>345</v>
       </c>
-      <c r="Z5" s="160"/>
-      <c r="AA5" s="160"/>
-      <c r="AB5" s="160"/>
-      <c r="AC5" s="160"/>
-      <c r="AD5" s="160"/>
-      <c r="AE5" s="160"/>
-      <c r="AF5" s="161" t="s">
+      <c r="Z5" s="165"/>
+      <c r="AA5" s="165"/>
+      <c r="AB5" s="165"/>
+      <c r="AC5" s="165"/>
+      <c r="AD5" s="165"/>
+      <c r="AE5" s="165"/>
+      <c r="AF5" s="166" t="s">
         <v>336</v>
       </c>
-      <c r="AG5" s="161"/>
-      <c r="AH5" s="161"/>
-      <c r="AI5" s="161"/>
-      <c r="AJ5" s="161"/>
-      <c r="AK5" s="161"/>
-      <c r="AL5" s="161"/>
+      <c r="AG5" s="166"/>
+      <c r="AH5" s="166"/>
+      <c r="AI5" s="166"/>
+      <c r="AJ5" s="166"/>
+      <c r="AK5" s="166"/>
+      <c r="AL5" s="166"/>
       <c r="DC5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:107" x14ac:dyDescent="0.25">
-      <c r="I6" s="163"/>
-      <c r="J6" s="164"/>
-      <c r="K6" s="164"/>
-      <c r="L6" s="164"/>
-      <c r="M6" s="164"/>
-      <c r="N6" s="164"/>
-      <c r="O6" s="164"/>
-      <c r="P6" s="165"/>
-      <c r="Q6" s="163"/>
-      <c r="R6" s="164"/>
-      <c r="S6" s="164"/>
-      <c r="T6" s="164"/>
-      <c r="U6" s="164"/>
-      <c r="V6" s="164"/>
-      <c r="W6" s="164"/>
-      <c r="X6" s="165"/>
+      <c r="I6" s="168"/>
+      <c r="J6" s="169"/>
+      <c r="K6" s="169"/>
+      <c r="L6" s="169"/>
+      <c r="M6" s="169"/>
+      <c r="N6" s="169"/>
+      <c r="O6" s="169"/>
+      <c r="P6" s="170"/>
+      <c r="Q6" s="168"/>
+      <c r="R6" s="169"/>
+      <c r="S6" s="169"/>
+      <c r="T6" s="169"/>
+      <c r="U6" s="169"/>
+      <c r="V6" s="169"/>
+      <c r="W6" s="169"/>
+      <c r="X6" s="170"/>
       <c r="Y6" s="147" t="s">
         <v>338</v>
       </c>
@@ -27735,7 +27807,7 @@
         <v>340</v>
       </c>
       <c r="AE6" s="147"/>
-      <c r="AF6" s="162" t="s">
+      <c r="AF6" s="167" t="s">
         <v>338</v>
       </c>
       <c r="AG6" s="143"/>
@@ -27785,15 +27857,15 @@
       <c r="M7" s="149"/>
       <c r="N7" s="149"/>
       <c r="O7" s="149"/>
-      <c r="P7" s="153"/>
-      <c r="Q7" s="154"/>
-      <c r="R7" s="155"/>
-      <c r="S7" s="155"/>
-      <c r="T7" s="155"/>
-      <c r="U7" s="155"/>
-      <c r="V7" s="155"/>
-      <c r="W7" s="155"/>
-      <c r="X7" s="156"/>
+      <c r="P7" s="161"/>
+      <c r="Q7" s="158"/>
+      <c r="R7" s="159"/>
+      <c r="S7" s="159"/>
+      <c r="T7" s="159"/>
+      <c r="U7" s="159"/>
+      <c r="V7" s="159"/>
+      <c r="W7" s="159"/>
+      <c r="X7" s="160"/>
       <c r="Y7" s="151" t="str">
         <f>IF(Y4=$DB$1,2+(TRUNC(H4/2)),"")&amp;IF(Y4=$DB$2,TRUNC(H4/3),"")&amp;IF(Y4=$DB$3,"-","")</f>
         <v/>
@@ -28343,26 +28415,26 @@
       <c r="BJ14" s="146"/>
     </row>
     <row r="15" spans="2:107" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="I15" s="157" t="s">
+      <c r="I15" s="162" t="s">
         <v>345</v>
       </c>
-      <c r="J15" s="158"/>
-      <c r="K15" s="158"/>
-      <c r="L15" s="158"/>
-      <c r="M15" s="158"/>
-      <c r="N15" s="158"/>
-      <c r="O15" s="158"/>
-      <c r="P15" s="159"/>
-      <c r="Q15" s="157" t="s">
+      <c r="J15" s="163"/>
+      <c r="K15" s="163"/>
+      <c r="L15" s="163"/>
+      <c r="M15" s="163"/>
+      <c r="N15" s="163"/>
+      <c r="O15" s="163"/>
+      <c r="P15" s="164"/>
+      <c r="Q15" s="162" t="s">
         <v>336</v>
       </c>
-      <c r="R15" s="158"/>
-      <c r="S15" s="158"/>
-      <c r="T15" s="158"/>
-      <c r="U15" s="158"/>
-      <c r="V15" s="158"/>
-      <c r="W15" s="158"/>
-      <c r="X15" s="159"/>
+      <c r="R15" s="163"/>
+      <c r="S15" s="163"/>
+      <c r="T15" s="163"/>
+      <c r="U15" s="163"/>
+      <c r="V15" s="163"/>
+      <c r="W15" s="163"/>
+      <c r="X15" s="164"/>
       <c r="Y15" s="172" t="s">
         <v>345</v>
       </c>
@@ -28383,22 +28455,22 @@
       <c r="AL15" s="177"/>
     </row>
     <row r="16" spans="2:107" x14ac:dyDescent="0.25">
-      <c r="I16" s="163"/>
-      <c r="J16" s="164"/>
-      <c r="K16" s="164"/>
-      <c r="L16" s="164"/>
-      <c r="M16" s="164"/>
-      <c r="N16" s="164"/>
-      <c r="O16" s="164"/>
-      <c r="P16" s="165"/>
-      <c r="Q16" s="163"/>
-      <c r="R16" s="164"/>
-      <c r="S16" s="164"/>
-      <c r="T16" s="164"/>
-      <c r="U16" s="164"/>
-      <c r="V16" s="164"/>
-      <c r="W16" s="164"/>
-      <c r="X16" s="165"/>
+      <c r="I16" s="168"/>
+      <c r="J16" s="169"/>
+      <c r="K16" s="169"/>
+      <c r="L16" s="169"/>
+      <c r="M16" s="169"/>
+      <c r="N16" s="169"/>
+      <c r="O16" s="169"/>
+      <c r="P16" s="170"/>
+      <c r="Q16" s="168"/>
+      <c r="R16" s="169"/>
+      <c r="S16" s="169"/>
+      <c r="T16" s="169"/>
+      <c r="U16" s="169"/>
+      <c r="V16" s="169"/>
+      <c r="W16" s="169"/>
+      <c r="X16" s="170"/>
       <c r="Y16" s="178" t="s">
         <v>338</v>
       </c>
@@ -28415,16 +28487,16 @@
       <c r="AF16" s="181" t="s">
         <v>338</v>
       </c>
-      <c r="AG16" s="170"/>
-      <c r="AH16" s="168" t="s">
+      <c r="AG16" s="157"/>
+      <c r="AH16" s="155" t="s">
         <v>339</v>
       </c>
-      <c r="AI16" s="169"/>
-      <c r="AJ16" s="170"/>
-      <c r="AK16" s="168" t="s">
+      <c r="AI16" s="156"/>
+      <c r="AJ16" s="157"/>
+      <c r="AK16" s="155" t="s">
         <v>340</v>
       </c>
-      <c r="AL16" s="170"/>
+      <c r="AL16" s="157"/>
     </row>
     <row r="17" spans="2:38" x14ac:dyDescent="0.25">
       <c r="I17" s="148" t="str">
@@ -28437,15 +28509,15 @@
       <c r="M17" s="149"/>
       <c r="N17" s="149"/>
       <c r="O17" s="149"/>
-      <c r="P17" s="153"/>
-      <c r="Q17" s="154"/>
-      <c r="R17" s="155"/>
-      <c r="S17" s="155"/>
-      <c r="T17" s="155"/>
-      <c r="U17" s="155"/>
-      <c r="V17" s="155"/>
-      <c r="W17" s="155"/>
-      <c r="X17" s="156"/>
+      <c r="P17" s="161"/>
+      <c r="Q17" s="158"/>
+      <c r="R17" s="159"/>
+      <c r="S17" s="159"/>
+      <c r="T17" s="159"/>
+      <c r="U17" s="159"/>
+      <c r="V17" s="159"/>
+      <c r="W17" s="159"/>
+      <c r="X17" s="160"/>
       <c r="Y17" s="171" t="str">
         <f>IF(Y14=$DB$1,2+(TRUNC(H14/2)),"")&amp;IF(Y14=$DB$2,TRUNC(H14/3),"")&amp;IF(Y14=$DB$3,"-","")</f>
         <v/>
@@ -28461,14 +28533,14 @@
         <f>IF(AI14=$DB$1,2+(TRUNC(H14/2)),"")&amp;IF(AI14=$DB$2,TRUNC(H14/3),"")&amp;IF(AI14=$DB$3,"-","")</f>
         <v/>
       </c>
-      <c r="AE17" s="153"/>
-      <c r="AF17" s="154"/>
-      <c r="AG17" s="156"/>
-      <c r="AH17" s="154"/>
-      <c r="AI17" s="155"/>
-      <c r="AJ17" s="156"/>
-      <c r="AK17" s="154"/>
-      <c r="AL17" s="156"/>
+      <c r="AE17" s="161"/>
+      <c r="AF17" s="158"/>
+      <c r="AG17" s="160"/>
+      <c r="AH17" s="158"/>
+      <c r="AI17" s="159"/>
+      <c r="AJ17" s="160"/>
+      <c r="AK17" s="158"/>
+      <c r="AL17" s="160"/>
     </row>
     <row r="18" spans="2:38" x14ac:dyDescent="0.25">
       <c r="AD18" s="205" t="s">
@@ -28484,46 +28556,46 @@
       <c r="AL18" s="207"/>
     </row>
     <row r="19" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="AD19" s="168" t="s">
+      <c r="AD19" s="155" t="s">
         <v>358</v>
       </c>
-      <c r="AE19" s="169"/>
-      <c r="AF19" s="169"/>
-      <c r="AG19" s="169"/>
-      <c r="AH19" s="169"/>
-      <c r="AI19" s="169"/>
-      <c r="AJ19" s="169"/>
-      <c r="AK19" s="169"/>
-      <c r="AL19" s="170"/>
+      <c r="AE19" s="156"/>
+      <c r="AF19" s="156"/>
+      <c r="AG19" s="156"/>
+      <c r="AH19" s="156"/>
+      <c r="AI19" s="156"/>
+      <c r="AJ19" s="156"/>
+      <c r="AK19" s="156"/>
+      <c r="AL19" s="157"/>
     </row>
     <row r="20" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="AD20" s="154"/>
-      <c r="AE20" s="155"/>
-      <c r="AF20" s="155"/>
-      <c r="AG20" s="155"/>
-      <c r="AH20" s="155"/>
-      <c r="AI20" s="155"/>
-      <c r="AJ20" s="155"/>
-      <c r="AK20" s="155"/>
-      <c r="AL20" s="156"/>
+      <c r="AD20" s="158"/>
+      <c r="AE20" s="159"/>
+      <c r="AF20" s="159"/>
+      <c r="AG20" s="159"/>
+      <c r="AH20" s="159"/>
+      <c r="AI20" s="159"/>
+      <c r="AJ20" s="159"/>
+      <c r="AK20" s="159"/>
+      <c r="AL20" s="160"/>
     </row>
     <row r="22" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="Y22" s="166" t="s">
+      <c r="Y22" s="153" t="s">
         <v>337</v>
       </c>
-      <c r="Z22" s="166"/>
-      <c r="AA22" s="166"/>
-      <c r="AB22" s="166"/>
-      <c r="AC22" s="166"/>
-      <c r="AD22" s="166"/>
-      <c r="AE22" s="166"/>
-      <c r="AF22" s="166"/>
-      <c r="AG22" s="166"/>
-      <c r="AH22" s="166"/>
-      <c r="AI22" s="166"/>
-      <c r="AJ22" s="166"/>
-      <c r="AK22" s="166"/>
-      <c r="AL22" s="167"/>
+      <c r="Z22" s="153"/>
+      <c r="AA22" s="153"/>
+      <c r="AB22" s="153"/>
+      <c r="AC22" s="153"/>
+      <c r="AD22" s="153"/>
+      <c r="AE22" s="153"/>
+      <c r="AF22" s="153"/>
+      <c r="AG22" s="153"/>
+      <c r="AH22" s="153"/>
+      <c r="AI22" s="153"/>
+      <c r="AJ22" s="153"/>
+      <c r="AK22" s="153"/>
+      <c r="AL22" s="154"/>
     </row>
     <row r="23" spans="2:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="144" t="s">
@@ -28616,62 +28688,62 @@
       <c r="AL24" s="139"/>
     </row>
     <row r="25" spans="2:38" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="I25" s="157" t="s">
+      <c r="I25" s="162" t="s">
         <v>345</v>
       </c>
-      <c r="J25" s="158"/>
-      <c r="K25" s="158"/>
-      <c r="L25" s="158"/>
-      <c r="M25" s="158"/>
-      <c r="N25" s="158"/>
-      <c r="O25" s="158"/>
-      <c r="P25" s="159"/>
-      <c r="Q25" s="157" t="s">
+      <c r="J25" s="163"/>
+      <c r="K25" s="163"/>
+      <c r="L25" s="163"/>
+      <c r="M25" s="163"/>
+      <c r="N25" s="163"/>
+      <c r="O25" s="163"/>
+      <c r="P25" s="164"/>
+      <c r="Q25" s="162" t="s">
         <v>336</v>
       </c>
-      <c r="R25" s="158"/>
-      <c r="S25" s="158"/>
-      <c r="T25" s="158"/>
-      <c r="U25" s="158"/>
-      <c r="V25" s="158"/>
-      <c r="W25" s="158"/>
-      <c r="X25" s="159"/>
-      <c r="Y25" s="160" t="s">
+      <c r="R25" s="163"/>
+      <c r="S25" s="163"/>
+      <c r="T25" s="163"/>
+      <c r="U25" s="163"/>
+      <c r="V25" s="163"/>
+      <c r="W25" s="163"/>
+      <c r="X25" s="164"/>
+      <c r="Y25" s="165" t="s">
         <v>345</v>
       </c>
-      <c r="Z25" s="160"/>
-      <c r="AA25" s="160"/>
-      <c r="AB25" s="160"/>
-      <c r="AC25" s="160"/>
-      <c r="AD25" s="160"/>
-      <c r="AE25" s="160"/>
-      <c r="AF25" s="161" t="s">
+      <c r="Z25" s="165"/>
+      <c r="AA25" s="165"/>
+      <c r="AB25" s="165"/>
+      <c r="AC25" s="165"/>
+      <c r="AD25" s="165"/>
+      <c r="AE25" s="165"/>
+      <c r="AF25" s="166" t="s">
         <v>336</v>
       </c>
-      <c r="AG25" s="161"/>
-      <c r="AH25" s="161"/>
-      <c r="AI25" s="161"/>
-      <c r="AJ25" s="161"/>
-      <c r="AK25" s="161"/>
-      <c r="AL25" s="161"/>
+      <c r="AG25" s="166"/>
+      <c r="AH25" s="166"/>
+      <c r="AI25" s="166"/>
+      <c r="AJ25" s="166"/>
+      <c r="AK25" s="166"/>
+      <c r="AL25" s="166"/>
     </row>
     <row r="26" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="I26" s="163"/>
-      <c r="J26" s="164"/>
-      <c r="K26" s="164"/>
-      <c r="L26" s="164"/>
-      <c r="M26" s="164"/>
-      <c r="N26" s="164"/>
-      <c r="O26" s="164"/>
-      <c r="P26" s="165"/>
-      <c r="Q26" s="163"/>
-      <c r="R26" s="164"/>
-      <c r="S26" s="164"/>
-      <c r="T26" s="164"/>
-      <c r="U26" s="164"/>
-      <c r="V26" s="164"/>
-      <c r="W26" s="164"/>
-      <c r="X26" s="165"/>
+      <c r="I26" s="168"/>
+      <c r="J26" s="169"/>
+      <c r="K26" s="169"/>
+      <c r="L26" s="169"/>
+      <c r="M26" s="169"/>
+      <c r="N26" s="169"/>
+      <c r="O26" s="169"/>
+      <c r="P26" s="170"/>
+      <c r="Q26" s="168"/>
+      <c r="R26" s="169"/>
+      <c r="S26" s="169"/>
+      <c r="T26" s="169"/>
+      <c r="U26" s="169"/>
+      <c r="V26" s="169"/>
+      <c r="W26" s="169"/>
+      <c r="X26" s="170"/>
       <c r="Y26" s="147" t="s">
         <v>338</v>
       </c>
@@ -28685,7 +28757,7 @@
         <v>340</v>
       </c>
       <c r="AE26" s="147"/>
-      <c r="AF26" s="162" t="s">
+      <c r="AF26" s="167" t="s">
         <v>338</v>
       </c>
       <c r="AG26" s="143"/>
@@ -28710,15 +28782,15 @@
       <c r="M27" s="149"/>
       <c r="N27" s="149"/>
       <c r="O27" s="149"/>
-      <c r="P27" s="153"/>
-      <c r="Q27" s="154"/>
-      <c r="R27" s="155"/>
-      <c r="S27" s="155"/>
-      <c r="T27" s="155"/>
-      <c r="U27" s="155"/>
-      <c r="V27" s="155"/>
-      <c r="W27" s="155"/>
-      <c r="X27" s="156"/>
+      <c r="P27" s="161"/>
+      <c r="Q27" s="158"/>
+      <c r="R27" s="159"/>
+      <c r="S27" s="159"/>
+      <c r="T27" s="159"/>
+      <c r="U27" s="159"/>
+      <c r="V27" s="159"/>
+      <c r="W27" s="159"/>
+      <c r="X27" s="160"/>
       <c r="Y27" s="151" t="str">
         <f>IF(Y24=$DB$1,2+(TRUNC(H24/2)),"")&amp;IF(Y24=$DB$2,TRUNC(H24/3),"")&amp;IF(Y24=$DB$3,"-","")</f>
         <v/>
@@ -28781,22 +28853,22 @@
       <c r="AL30" s="152"/>
     </row>
     <row r="32" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="Y32" s="166" t="s">
+      <c r="Y32" s="153" t="s">
         <v>337</v>
       </c>
-      <c r="Z32" s="166"/>
-      <c r="AA32" s="166"/>
-      <c r="AB32" s="166"/>
-      <c r="AC32" s="166"/>
-      <c r="AD32" s="166"/>
-      <c r="AE32" s="166"/>
-      <c r="AF32" s="166"/>
-      <c r="AG32" s="166"/>
-      <c r="AH32" s="166"/>
-      <c r="AI32" s="166"/>
-      <c r="AJ32" s="166"/>
-      <c r="AK32" s="166"/>
-      <c r="AL32" s="167"/>
+      <c r="Z32" s="153"/>
+      <c r="AA32" s="153"/>
+      <c r="AB32" s="153"/>
+      <c r="AC32" s="153"/>
+      <c r="AD32" s="153"/>
+      <c r="AE32" s="153"/>
+      <c r="AF32" s="153"/>
+      <c r="AG32" s="153"/>
+      <c r="AH32" s="153"/>
+      <c r="AI32" s="153"/>
+      <c r="AJ32" s="153"/>
+      <c r="AK32" s="153"/>
+      <c r="AL32" s="154"/>
     </row>
     <row r="33" spans="2:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="144" t="s">
@@ -28889,62 +28961,62 @@
       <c r="AL34" s="139"/>
     </row>
     <row r="35" spans="2:38" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="I35" s="157" t="s">
+      <c r="I35" s="162" t="s">
         <v>345</v>
       </c>
-      <c r="J35" s="158"/>
-      <c r="K35" s="158"/>
-      <c r="L35" s="158"/>
-      <c r="M35" s="158"/>
-      <c r="N35" s="158"/>
-      <c r="O35" s="158"/>
-      <c r="P35" s="159"/>
-      <c r="Q35" s="157" t="s">
+      <c r="J35" s="163"/>
+      <c r="K35" s="163"/>
+      <c r="L35" s="163"/>
+      <c r="M35" s="163"/>
+      <c r="N35" s="163"/>
+      <c r="O35" s="163"/>
+      <c r="P35" s="164"/>
+      <c r="Q35" s="162" t="s">
         <v>336</v>
       </c>
-      <c r="R35" s="158"/>
-      <c r="S35" s="158"/>
-      <c r="T35" s="158"/>
-      <c r="U35" s="158"/>
-      <c r="V35" s="158"/>
-      <c r="W35" s="158"/>
-      <c r="X35" s="159"/>
-      <c r="Y35" s="160" t="s">
+      <c r="R35" s="163"/>
+      <c r="S35" s="163"/>
+      <c r="T35" s="163"/>
+      <c r="U35" s="163"/>
+      <c r="V35" s="163"/>
+      <c r="W35" s="163"/>
+      <c r="X35" s="164"/>
+      <c r="Y35" s="165" t="s">
         <v>345</v>
       </c>
-      <c r="Z35" s="160"/>
-      <c r="AA35" s="160"/>
-      <c r="AB35" s="160"/>
-      <c r="AC35" s="160"/>
-      <c r="AD35" s="160"/>
-      <c r="AE35" s="160"/>
-      <c r="AF35" s="161" t="s">
+      <c r="Z35" s="165"/>
+      <c r="AA35" s="165"/>
+      <c r="AB35" s="165"/>
+      <c r="AC35" s="165"/>
+      <c r="AD35" s="165"/>
+      <c r="AE35" s="165"/>
+      <c r="AF35" s="166" t="s">
         <v>336</v>
       </c>
-      <c r="AG35" s="161"/>
-      <c r="AH35" s="161"/>
-      <c r="AI35" s="161"/>
-      <c r="AJ35" s="161"/>
-      <c r="AK35" s="161"/>
-      <c r="AL35" s="161"/>
+      <c r="AG35" s="166"/>
+      <c r="AH35" s="166"/>
+      <c r="AI35" s="166"/>
+      <c r="AJ35" s="166"/>
+      <c r="AK35" s="166"/>
+      <c r="AL35" s="166"/>
     </row>
     <row r="36" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="I36" s="163"/>
-      <c r="J36" s="164"/>
-      <c r="K36" s="164"/>
-      <c r="L36" s="164"/>
-      <c r="M36" s="164"/>
-      <c r="N36" s="164"/>
-      <c r="O36" s="164"/>
-      <c r="P36" s="165"/>
-      <c r="Q36" s="163"/>
-      <c r="R36" s="164"/>
-      <c r="S36" s="164"/>
-      <c r="T36" s="164"/>
-      <c r="U36" s="164"/>
-      <c r="V36" s="164"/>
-      <c r="W36" s="164"/>
-      <c r="X36" s="165"/>
+      <c r="I36" s="168"/>
+      <c r="J36" s="169"/>
+      <c r="K36" s="169"/>
+      <c r="L36" s="169"/>
+      <c r="M36" s="169"/>
+      <c r="N36" s="169"/>
+      <c r="O36" s="169"/>
+      <c r="P36" s="170"/>
+      <c r="Q36" s="168"/>
+      <c r="R36" s="169"/>
+      <c r="S36" s="169"/>
+      <c r="T36" s="169"/>
+      <c r="U36" s="169"/>
+      <c r="V36" s="169"/>
+      <c r="W36" s="169"/>
+      <c r="X36" s="170"/>
       <c r="Y36" s="147" t="s">
         <v>338</v>
       </c>
@@ -28958,7 +29030,7 @@
         <v>340</v>
       </c>
       <c r="AE36" s="147"/>
-      <c r="AF36" s="162" t="s">
+      <c r="AF36" s="167" t="s">
         <v>338</v>
       </c>
       <c r="AG36" s="143"/>
@@ -28983,15 +29055,15 @@
       <c r="M37" s="149"/>
       <c r="N37" s="149"/>
       <c r="O37" s="149"/>
-      <c r="P37" s="153"/>
-      <c r="Q37" s="154"/>
-      <c r="R37" s="155"/>
-      <c r="S37" s="155"/>
-      <c r="T37" s="155"/>
-      <c r="U37" s="155"/>
-      <c r="V37" s="155"/>
-      <c r="W37" s="155"/>
-      <c r="X37" s="156"/>
+      <c r="P37" s="161"/>
+      <c r="Q37" s="158"/>
+      <c r="R37" s="159"/>
+      <c r="S37" s="159"/>
+      <c r="T37" s="159"/>
+      <c r="U37" s="159"/>
+      <c r="V37" s="159"/>
+      <c r="W37" s="159"/>
+      <c r="X37" s="160"/>
       <c r="Y37" s="151" t="str">
         <f>IF(Y34=$DB$1,2+(TRUNC(H34/2)),"")&amp;IF(Y34=$DB$2,TRUNC(H34/3),"")&amp;IF(Y34=$DB$3,"-","")</f>
         <v/>

</xml_diff>